<commit_message>
search bug fix (included key={})
</commit_message>
<xml_diff>
--- a/public/assets/champ_names.xlsx
+++ b/public/assets/champ_names.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Constantine\Desktop\lol picker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Constantine\Desktop\app\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>AATROX</t>
   </si>
@@ -484,6 +484,15 @@
   </si>
   <si>
     <t>ZYRA</t>
+  </si>
+  <si>
+    <t>AKSHAN</t>
+  </si>
+  <si>
+    <t>champion</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -822,789 +831,1270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A155"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>